<commit_message>
Added title and modified shifts
</commit_message>
<xml_diff>
--- a/Excel docs/Schedule-2019-09-24.xlsx
+++ b/Excel docs/Schedule-2019-09-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\engcf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Documents/engcf/Excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEA6904-50E8-4627-A0A5-B75C02885A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F994C-F33B-974C-8540-AE17167349D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly - Career Fair" sheetId="1" r:id="rId1"/>
@@ -819,7 +819,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -827,7 +827,7 @@
     <col min="5" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="ZY1" s="2"/>
       <c r="ZZ1" s="2"/>
     </row>
-    <row r="2" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>16</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>36</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>37</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>40</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>44</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>22</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>46</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>49</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>51</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>40</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>52</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>53</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>13</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>55</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>57</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>14</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>58</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>43</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>40</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>59</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>60</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>61</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>62</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>63</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>64</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>65</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>66</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
         <v>67</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>68</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
         <v>10</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>69</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>11</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>70</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
         <v>10</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>71</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>43</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>72</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>74</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>14</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>75</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>76</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>77</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>78</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>79</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>48</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>80</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>81</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>82</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>83</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>84</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>85</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>86</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>87</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>50</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>88</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>89</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>90</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>91</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
         <v>14</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>93</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>14</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>94</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>95</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
         <v>11</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>96</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
         <v>54</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>97</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>54</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>99</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>27</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>103</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>104</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
         <v>37</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>105</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C110" t="s">
         <v>22</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
         <v>36</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C112" t="s">
         <v>54</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>106</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>107</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>108</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>109</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>110</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>111</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>112</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>113</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
         <v>36</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
         <v>67</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>114</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>115</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>116</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>118</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C127" t="s">
         <v>34</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>119</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>120</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>121</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>122</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
         <v>11</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>123</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>124</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
         <v>36</v>
       </c>
@@ -4116,11 +4116,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>125</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>126</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -4163,7 +4163,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>128</v>
       </c>
@@ -4185,22 +4185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="117" workbookViewId="0">
-      <selection activeCell="H147" sqref="H147"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
@@ -4256,7 +4256,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43732.333333333001</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43732.375</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43732.375</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43732.375</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43732.375</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43732.375</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43732.375</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>43732.375</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>43732.375</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>43732.375</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>43732.375</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>43732.375</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43732.375</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>43732.375</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>43732.5</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>43732.5</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>43732.5</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>43732.5</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>43732.5</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>43732.5</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>43732.5</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>43732.5</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>43732.5</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>43732.5</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>43732.5</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>43732.5</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>43732.5</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>43732.5</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>43732.5</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>43732.5</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>43732.5</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>43732.5</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6688,12 +6688,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>43732.541666666999</v>
       </c>
       <c r="B73" t="s">
         <v>140</v>
+      </c>
+      <c r="C73">
+        <v>490227758</v>
       </c>
       <c r="D73" t="s">
         <v>22</v>
@@ -6722,7 +6725,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6756,7 +6759,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6790,7 +6793,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6824,7 +6827,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6858,7 +6861,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6892,7 +6895,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6926,7 +6929,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6960,7 +6963,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6994,7 +6997,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7028,7 +7031,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7062,7 +7065,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7096,7 +7099,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7130,7 +7133,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7164,7 +7167,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7198,7 +7201,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7232,7 +7235,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7266,7 +7269,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7300,7 +7303,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7334,7 +7337,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7368,7 +7371,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7402,7 +7405,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7436,7 +7439,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7470,7 +7473,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7504,7 +7507,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7538,7 +7541,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7572,7 +7575,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7606,7 +7609,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7640,7 +7643,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7674,7 +7677,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7708,7 +7711,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7742,7 +7745,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>43732.625</v>
       </c>
@@ -7776,7 +7779,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>43732.625</v>
       </c>
@@ -7810,7 +7813,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>43732.625</v>
       </c>
@@ -7844,7 +7847,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>43732.625</v>
       </c>
@@ -7878,7 +7881,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>43732.625</v>
       </c>
@@ -7912,7 +7915,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>43732.625</v>
       </c>
@@ -7946,7 +7949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>43732.625</v>
       </c>
@@ -7980,7 +7983,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>43732.625</v>
       </c>
@@ -8014,7 +8017,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>43732.625</v>
       </c>
@@ -8048,7 +8051,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>43732.625</v>
       </c>
@@ -8082,7 +8085,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>43732.625</v>
       </c>
@@ -8116,7 +8119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>43732.625</v>
       </c>
@@ -8150,7 +8153,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>43732.625</v>
       </c>
@@ -8184,7 +8187,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>43732.625</v>
       </c>
@@ -8218,7 +8221,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>43732.625</v>
       </c>
@@ -8252,7 +8255,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>43732.625</v>
       </c>
@@ -8286,7 +8289,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>43732.625</v>
       </c>
@@ -8320,7 +8323,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8357,7 +8360,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8391,7 +8394,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8425,7 +8428,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8459,7 +8462,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8493,7 +8496,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8527,7 +8530,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8561,7 +8564,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8595,7 +8598,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8629,7 +8632,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8663,7 +8666,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8697,7 +8700,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8731,7 +8734,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8765,7 +8768,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8799,7 +8802,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8833,7 +8836,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8867,7 +8870,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8901,7 +8904,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8935,7 +8938,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -8972,7 +8975,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9006,7 +9009,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9040,7 +9043,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9074,7 +9077,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9108,7 +9111,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9142,7 +9145,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9176,7 +9179,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9210,7 +9213,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9244,7 +9247,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9278,7 +9281,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9312,7 +9315,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9346,7 +9349,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9380,7 +9383,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9417,7 +9420,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>

</xml_diff>

<commit_message>
refactored for new implementation
</commit_message>
<xml_diff>
--- a/Excel docs/Schedule-2019-09-24.xlsx
+++ b/Excel docs/Schedule-2019-09-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Documents/engcf/Excel docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\engcf\Excel docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1F994C-F33B-974C-8540-AE17167349D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CF9016-DF31-4B08-8E10-5074CAF5D9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly - Career Fair" sheetId="1" r:id="rId1"/>
@@ -819,7 +819,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -827,7 +827,7 @@
     <col min="5" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:702" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="ZY1" s="2"/>
       <c r="ZZ1" s="2"/>
     </row>
-    <row r="2" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:702" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>16</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:702" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:702" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>36</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>37</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>40</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>44</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>22</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>46</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>49</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>51</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>40</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>52</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>53</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>13</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>55</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>57</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>14</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>58</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>43</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>40</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>59</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>60</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>61</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>62</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>63</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>64</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>65</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>66</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>67</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>68</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>10</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>69</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>11</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>70</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>10</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>71</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>43</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>72</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>74</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
         <v>14</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>75</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>76</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>77</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>78</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>79</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
         <v>48</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>80</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>81</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>82</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>83</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>84</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>85</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>86</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>87</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>50</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>88</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>89</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>90</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>91</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C90" t="s">
         <v>14</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>93</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>14</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>94</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>95</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>11</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>96</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C97" t="s">
         <v>54</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>97</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C99" t="s">
         <v>54</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>99</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
         <v>27</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>103</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>104</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
         <v>37</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>105</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C110" t="s">
         <v>22</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C111" t="s">
         <v>36</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C112" t="s">
         <v>54</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>106</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>107</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>108</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>109</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>110</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>111</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>112</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>113</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C121" t="s">
         <v>36</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C122" t="s">
         <v>67</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>114</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>115</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>116</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>118</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C127" t="s">
         <v>34</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>119</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>120</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>121</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>122</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C132" t="s">
         <v>11</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>123</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>124</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C135" t="s">
         <v>36</v>
       </c>
@@ -4116,11 +4116,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>125</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>126</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -4163,7 +4163,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>128</v>
       </c>
@@ -4185,22 +4185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
@@ -4256,7 +4256,7 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43732.333333333001</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43732.375</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43732.375</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43732.375</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43732.375</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43732.375</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43732.375</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43732.375</v>
       </c>
@@ -4534,7 +4534,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43732.375</v>
       </c>
@@ -4568,7 +4568,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43732.375</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43732.375</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43732.375</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43732.375</v>
       </c>
@@ -4704,7 +4704,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43732.375</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5118,7 +5118,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5631,7 +5631,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5801,7 +5801,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43732.5</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43732.5</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>43732.5</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43732.5</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43732.5</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>43732.5</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>43732.5</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43732.5</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43732.5</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>43732.5</v>
       </c>
@@ -6212,7 +6212,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43732.5</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>43732.5</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>43732.5</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43732.5</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>43732.5</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>43732.5</v>
       </c>
@@ -6416,7 +6416,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>43732.5</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>43732.5</v>
       </c>
@@ -6484,7 +6484,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6620,7 +6620,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6654,7 +6654,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6759,7 +6759,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6793,7 +6793,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6861,7 +6861,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6963,7 +6963,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7133,7 +7133,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7235,7 +7235,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7371,7 +7371,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7575,7 +7575,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7609,7 +7609,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7677,7 +7677,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7711,7 +7711,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>43732.625</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>43732.625</v>
       </c>
@@ -7813,7 +7813,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>43732.625</v>
       </c>
@@ -7847,7 +7847,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>43732.625</v>
       </c>
@@ -7881,7 +7881,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>43732.625</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>43732.625</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>43732.625</v>
       </c>
@@ -7983,7 +7983,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>43732.625</v>
       </c>
@@ -8017,7 +8017,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>43732.625</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>43732.625</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>43732.625</v>
       </c>
@@ -8119,7 +8119,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>43732.625</v>
       </c>
@@ -8153,7 +8153,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>43732.625</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>43732.625</v>
       </c>
@@ -8221,7 +8221,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>43732.625</v>
       </c>
@@ -8255,7 +8255,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>43732.625</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>43732.625</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8360,12 +8360,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>43732.666666666999</v>
       </c>
       <c r="B122" t="s">
         <v>33</v>
+      </c>
+      <c r="C122">
+        <v>490227758</v>
       </c>
       <c r="D122" t="s">
         <v>34</v>
@@ -8394,7 +8397,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8428,7 +8431,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8462,7 +8465,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8496,7 +8499,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8530,7 +8533,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8564,7 +8567,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8598,7 +8601,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8632,7 +8635,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8666,7 +8669,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8700,7 +8703,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8734,7 +8737,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8768,7 +8771,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8802,7 +8805,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8836,7 +8839,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8870,7 +8873,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8904,7 +8907,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8938,7 +8941,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -8975,7 +8978,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9009,7 +9012,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9043,7 +9046,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9077,7 +9080,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9111,7 +9114,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9145,7 +9148,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9179,7 +9182,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9213,7 +9216,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9247,7 +9250,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9281,7 +9284,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9315,7 +9318,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9349,7 +9352,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9383,7 +9386,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9420,7 +9423,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>

</xml_diff>

<commit_message>
Reorganized folder - archived old .js files
</commit_message>
<xml_diff>
--- a/Excel docs/Schedule-2019-09-24.xlsx
+++ b/Excel docs/Schedule-2019-09-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\engcf\Excel docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mvandewille/Documents/engcf/Excel docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2E899D-C489-427D-A8A0-BEABAC0729DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA9BAD0-DD41-3B44-A573-8063E82761D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly - Career Fair" sheetId="1" r:id="rId1"/>
@@ -815,11 +815,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ZZ140"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="190" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="190" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="18" customWidth="1"/>
@@ -827,7 +827,7 @@
     <col min="5" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:702" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +1547,7 @@
       <c r="ZY1" s="2"/>
       <c r="ZZ1" s="2"/>
     </row>
-    <row r="2" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>19</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:702" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>16</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:702" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:702" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>26</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>30</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>31</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>32</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>36</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>37</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>39</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>42</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>40</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>44</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>22</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>14</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>46</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>49</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>51</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>40</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>52</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>53</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>13</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>55</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>57</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>14</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>58</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>43</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>40</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>59</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>60</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>61</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>62</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>63</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>64</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>65</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>66</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
         <v>67</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>68</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
         <v>10</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>69</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
         <v>11</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>70</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
         <v>10</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>71</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>43</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>72</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>74</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>14</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>75</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>76</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>77</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>78</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>79</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>48</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>80</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>81</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>82</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>83</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>84</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>85</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>86</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>87</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>50</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>88</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>89</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>90</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>91</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>92</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
         <v>14</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>93</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>14</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>94</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>95</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
         <v>11</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>96</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C97" t="s">
         <v>54</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>97</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C99" t="s">
         <v>54</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>98</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>99</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>100</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>101</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>102</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C105" t="s">
         <v>27</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>103</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>104</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C108" t="s">
         <v>37</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>105</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C110" t="s">
         <v>22</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
         <v>36</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C112" t="s">
         <v>54</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>106</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>107</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>108</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>109</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>110</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>111</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>112</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>113</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
         <v>36</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
         <v>67</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>114</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>115</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>116</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>118</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C127" t="s">
         <v>34</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>119</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>120</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>121</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>122</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C132" t="s">
         <v>11</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>123</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>124</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C135" t="s">
         <v>36</v>
       </c>
@@ -4116,11 +4116,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>125</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>126</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>127</v>
       </c>
@@ -4163,7 +4163,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>128</v>
       </c>
@@ -4185,22 +4185,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C152"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
@@ -4256,12 +4256,15 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43732.333333333001</v>
       </c>
       <c r="B2" t="s">
         <v>140</v>
+      </c>
+      <c r="C2">
+        <v>490227758</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
@@ -4290,7 +4293,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43732.375</v>
       </c>
@@ -4324,7 +4327,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43732.375</v>
       </c>
@@ -4358,7 +4361,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43732.375</v>
       </c>
@@ -4392,7 +4395,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43732.375</v>
       </c>
@@ -4426,7 +4429,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43732.375</v>
       </c>
@@ -4460,7 +4463,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43732.375</v>
       </c>
@@ -4494,7 +4497,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>43732.375</v>
       </c>
@@ -4528,7 +4531,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>43732.375</v>
       </c>
@@ -4562,7 +4565,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>43732.375</v>
       </c>
@@ -4596,7 +4599,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>43732.375</v>
       </c>
@@ -4630,7 +4633,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>43732.375</v>
       </c>
@@ -4664,7 +4667,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43732.375</v>
       </c>
@@ -4698,7 +4701,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>43732.375</v>
       </c>
@@ -4732,7 +4735,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4766,7 +4769,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4800,7 +4803,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4834,7 +4837,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4868,7 +4871,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4902,7 +4905,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4936,7 +4939,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -4970,7 +4973,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5004,7 +5007,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5038,7 +5041,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>43732.416666666999</v>
       </c>
@@ -5072,7 +5075,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5106,7 +5109,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5140,7 +5143,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5174,7 +5177,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5208,7 +5211,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5242,7 +5245,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5276,7 +5279,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5310,7 +5313,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5344,7 +5347,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5378,7 +5381,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5412,7 +5415,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5446,7 +5449,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5480,7 +5483,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5514,7 +5517,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5548,7 +5551,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5582,7 +5585,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5616,7 +5619,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5650,7 +5653,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5684,7 +5687,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5718,7 +5721,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5752,7 +5755,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5786,7 +5789,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5820,7 +5823,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>43732.458333333001</v>
       </c>
@@ -5854,7 +5857,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>43732.5</v>
       </c>
@@ -5888,7 +5891,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>43732.5</v>
       </c>
@@ -5922,7 +5925,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>43732.5</v>
       </c>
@@ -5956,7 +5959,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>43732.5</v>
       </c>
@@ -5990,7 +5993,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>43732.5</v>
       </c>
@@ -6024,7 +6027,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>43732.5</v>
       </c>
@@ -6058,7 +6061,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>43732.5</v>
       </c>
@@ -6092,7 +6095,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>43732.5</v>
       </c>
@@ -6126,7 +6129,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>43732.5</v>
       </c>
@@ -6160,7 +6163,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>43732.5</v>
       </c>
@@ -6194,7 +6197,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>43732.5</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>43732.5</v>
       </c>
@@ -6262,7 +6265,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>43732.5</v>
       </c>
@@ -6296,7 +6299,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>43732.5</v>
       </c>
@@ -6330,7 +6333,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>43732.5</v>
       </c>
@@ -6364,7 +6367,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>43732.5</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>43732.5</v>
       </c>
@@ -6432,7 +6435,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>43732.5</v>
       </c>
@@ -6466,7 +6469,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6500,7 +6503,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6534,7 +6537,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6568,7 +6571,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6602,7 +6605,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6636,7 +6639,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6670,7 +6673,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6704,7 +6707,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6738,7 +6741,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6772,7 +6775,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6806,7 +6809,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6840,7 +6843,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6874,7 +6877,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6908,7 +6911,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6942,7 +6945,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -6976,7 +6979,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7010,7 +7013,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7044,7 +7047,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7078,7 +7081,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>43732.541666666999</v>
       </c>
@@ -7112,7 +7115,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7146,7 +7149,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7180,12 +7183,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>43732.583333333001</v>
       </c>
       <c r="B88" t="s">
         <v>140</v>
+      </c>
+      <c r="C88">
+        <v>490227758</v>
       </c>
       <c r="D88" t="s">
         <v>36</v>
@@ -7214,7 +7220,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7248,7 +7254,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7282,7 +7288,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7316,7 +7322,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7350,7 +7356,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7384,7 +7390,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7418,7 +7424,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7452,7 +7458,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7486,7 +7492,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7520,7 +7526,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7554,7 +7560,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7588,7 +7594,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7622,7 +7628,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7656,7 +7662,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7690,7 +7696,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>43732.583333333001</v>
       </c>
@@ -7724,7 +7730,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>43732.625</v>
       </c>
@@ -7758,7 +7764,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>43732.625</v>
       </c>
@@ -7792,7 +7798,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>43732.625</v>
       </c>
@@ -7826,7 +7832,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>43732.625</v>
       </c>
@@ -7860,7 +7866,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>43732.625</v>
       </c>
@@ -7894,7 +7900,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>43732.625</v>
       </c>
@@ -7928,7 +7934,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>43732.625</v>
       </c>
@@ -7962,7 +7968,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>43732.625</v>
       </c>
@@ -7996,7 +8002,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>43732.625</v>
       </c>
@@ -8030,7 +8036,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>43732.625</v>
       </c>
@@ -8064,7 +8070,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>43732.625</v>
       </c>
@@ -8098,7 +8104,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>43732.625</v>
       </c>
@@ -8132,7 +8138,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>43732.625</v>
       </c>
@@ -8166,7 +8172,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>43732.625</v>
       </c>
@@ -8200,7 +8206,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>43732.625</v>
       </c>
@@ -8234,12 +8240,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>43732.625</v>
       </c>
       <c r="B119" t="s">
         <v>140</v>
+      </c>
+      <c r="C119">
+        <v>490227758</v>
       </c>
       <c r="D119" t="s">
         <v>54</v>
@@ -8268,7 +8277,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>43732.625</v>
       </c>
@@ -8302,7 +8311,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8336,7 +8345,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8370,7 +8379,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8404,7 +8413,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8438,7 +8447,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8472,7 +8481,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8506,7 +8515,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8540,7 +8549,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8574,7 +8583,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8608,7 +8617,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8642,7 +8651,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8676,7 +8685,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8710,7 +8719,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8744,7 +8753,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8778,7 +8787,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8812,7 +8821,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8846,7 +8855,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8880,7 +8889,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>43732.666666666999</v>
       </c>
@@ -8914,7 +8923,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -8948,7 +8957,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -8982,7 +8991,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9016,7 +9025,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9050,7 +9059,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9084,7 +9093,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9118,7 +9127,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9152,7 +9161,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9186,7 +9195,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9220,7 +9229,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9254,7 +9263,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9288,7 +9297,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9322,7 +9331,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9356,7 +9365,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>43732.708333333001</v>
       </c>
@@ -9390,7 +9399,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" s="4"/>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>

</xml_diff>